<commit_message>
trucos y links de apoyo
</commit_message>
<xml_diff>
--- a/medidas.xlsx
+++ b/medidas.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Herramientas_WEB_git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B44115F6-9B74-42BA-939D-5303D749F1D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E9E21F3-67A7-441F-B730-6B10015A3172}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1995" yWindow="2415" windowWidth="15375" windowHeight="7875" xr2:uid="{BDA472F8-B5E3-4ADA-BF62-4124C1968C6C}"/>
+    <workbookView xWindow="3885" yWindow="2340" windowWidth="15375" windowHeight="7875" xr2:uid="{BDA472F8-B5E3-4ADA-BF62-4124C1968C6C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="FUENTE" sheetId="1" r:id="rId1"/>
+    <sheet name="lemento" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -24,9 +25,95 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>1em</t>
+  </si>
+  <si>
+    <t>PIXELES</t>
+  </si>
+  <si>
+    <t>EM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EM </t>
+  </si>
+  <si>
+    <t>en PIXELES</t>
+  </si>
+  <si>
+    <t>PADRE</t>
+  </si>
+  <si>
+    <t>HIJO</t>
+  </si>
+  <si>
+    <t>NIETO</t>
+  </si>
+  <si>
+    <t>FUENTE</t>
+  </si>
+  <si>
+    <t>PIXLES</t>
+  </si>
+  <si>
+    <t>a    EM</t>
+  </si>
+  <si>
+    <t>PIXEL</t>
+  </si>
+  <si>
+    <t>RESULTADO</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>H3</t>
+  </si>
+  <si>
+    <t>H4</t>
+  </si>
+  <si>
+    <t>H5</t>
+  </si>
+  <si>
+    <t>H6</t>
+  </si>
+  <si>
+    <t>DIV</t>
+  </si>
+  <si>
+    <t>ELEMENTO</t>
+  </si>
+  <si>
+    <t>8px</t>
+  </si>
+  <si>
+    <t>font-size</t>
+  </si>
+  <si>
+    <t>todos a 16px</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -34,16 +121,62 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -51,12 +184,152 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,12 +644,425 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C43417F-58C3-4C21-B2AE-7D848F15D9E0}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="9" width="11.42578125" style="6"/>
+    <col min="10" max="16384" width="11.42578125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9">
+        <v>16</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="D4" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="11"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="14">
+        <v>1.25</v>
+      </c>
+      <c r="B6" s="15">
+        <f>A6*B2</f>
+        <v>20</v>
+      </c>
+      <c r="D6" s="16">
+        <v>16</v>
+      </c>
+      <c r="E6" s="15">
+        <f>D6/B2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C7" s="18"/>
+      <c r="D7" s="13"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="D8" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="11"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="14">
+        <v>1.25</v>
+      </c>
+      <c r="B10" s="17">
+        <f>A10*B6</f>
+        <v>25</v>
+      </c>
+      <c r="D10" s="14">
+        <v>16</v>
+      </c>
+      <c r="E10" s="15">
+        <f>D10/D6</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="11"/>
+      <c r="D12" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="11"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="14">
+        <v>1.25</v>
+      </c>
+      <c r="B14" s="15">
+        <f>A14*B10</f>
+        <v>31.25</v>
+      </c>
+      <c r="D14" s="14">
+        <v>18</v>
+      </c>
+      <c r="E14" s="15">
+        <f>D14/D10</f>
+        <v>1.125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="14">
+        <v>20</v>
+      </c>
+      <c r="B17" s="14">
+        <v>1.25</v>
+      </c>
+      <c r="C17" s="15">
+        <f>A17*B17</f>
+        <v>25</v>
+      </c>
+      <c r="D17" s="13"/>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="7">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D12:E12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED106952-196A-42AA-9985-C106F08DDA84}">
+  <dimension ref="A2:F23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" style="19"/>
+    <col min="3" max="3" width="9.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="21">
+        <v>16</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2">
+        <v>32</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="2">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="2">
+        <v>24</v>
+      </c>
+      <c r="C5" s="1">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2">
+        <v>16.5</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="25"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2">
+        <v>18.72</v>
+      </c>
+      <c r="C6" s="1">
+        <v>14</v>
+      </c>
+      <c r="D6" s="22">
+        <v>16.38</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="20">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="2">
+        <v>13.28</v>
+      </c>
+      <c r="C8" s="1">
+        <v>19</v>
+      </c>
+      <c r="D8" s="2">
+        <v>15.77</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="2">
+        <v>10.72</v>
+      </c>
+      <c r="C9" s="1">
+        <v>24</v>
+      </c>
+      <c r="D9" s="2">
+        <v>16.079999999999998</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="20">
+        <v>16</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>